<commit_message>
pruebo <p> en comment en el excel
</commit_message>
<xml_diff>
--- a/data/web-repositorio.xlsx
+++ b/data/web-repositorio.xlsx
@@ -283,7 +283,7 @@
     <t xml:space="preserve">Madera Cuadro Virgen María Pasta Piedra-2-</t>
   </si>
   <si>
-    <t xml:space="preserve">Virgen María en un diseño infantil. Pintada y modelada a mano en Pasta Piedra. 32x26 cm 1 cm grosor de la madera</t>
+    <t xml:space="preserve">Virgen María en un diseño infantil. Pintada y modelada a mano en Pasta Piedra. &lt;p&gt;32x26 cm 1 cm grosor de la madera&lt;/p&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">..\..\Pictures\A TRABAJOS WEB\Madera\CUADROS PASTA PIEDRA\Madera Cuadro Virgen María Pasta Piedra -2.jpg</t>
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Velas colores y aromas
Cambié vela de rosas por una de manzanas y cambié stock
</commit_message>
<xml_diff>
--- a/data/web-repositorio.xlsx
+++ b/data/web-repositorio.xlsx
@@ -335,18 +335,9 @@
     <t>..\..\Pictures\A TRABAJOS WEB\VELAS\CERA DE ABEJAS\Vela Cera de abeja chica.jpg</t>
   </si>
   <si>
-    <t>Velas Colores y Aromas -ROSAS-</t>
-  </si>
-  <si>
-    <t>vela colores y aromas rosas</t>
-  </si>
-  <si>
     <t>Elaboradas con parafina, colores y esencias perfumadas. 4,2x12 cm</t>
   </si>
   <si>
-    <t>..\..\Pictures\A TRABAJOS WEB\VELAS\COLORES Y AROMAS\Colores y aromas Rosas.jpg</t>
-  </si>
-  <si>
     <t>Cerámica Rosario engarzados (perfume de Rosas con cajita)</t>
   </si>
   <si>
@@ -450,6 +441,15 @@
   </si>
   <si>
     <t>..\Pictures\A TRABAJOS WEB\VARIOS\alfajores.jpg</t>
+  </si>
+  <si>
+    <t>vela colores y aromas manzana</t>
+  </si>
+  <si>
+    <t>..\..\Pictures\A TRABAJOS WEB\VELAS\COLORES Y AROMAS\coloresyaromasmanzana.jpg</t>
+  </si>
+  <si>
+    <t>Velas Colores y Aromas -Manzana-</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +560,12 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -701,11 +707,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -847,6 +850,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3"/>
@@ -1113,1067 +1120,1067 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="78.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="78.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="5"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="5"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="15">
-        <v>1</v>
-      </c>
-      <c r="C4" s="16">
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
         <v>2500</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>20</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="20"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15">
         <v>16000</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>90</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="24"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="25">
         <v>100</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>1200</v>
       </c>
-      <c r="D6" s="27">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28" t="s">
+      <c r="D6" s="26">
+        <v>1</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="25">
         <v>100</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>1200</v>
       </c>
-      <c r="D7" s="30">
-        <v>1</v>
-      </c>
-      <c r="E7" s="28" t="s">
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="25">
         <v>100</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <v>2000</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <v>2</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="5"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="26">
-        <v>1</v>
-      </c>
-      <c r="C9" s="27">
+      <c r="B9" s="25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26">
         <v>1200</v>
       </c>
-      <c r="D9" s="27">
-        <v>1</v>
-      </c>
-      <c r="E9" s="28" t="s">
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="13"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="26">
-        <v>1</v>
-      </c>
-      <c r="C10" s="27">
+      <c r="B10" s="25">
+        <v>1</v>
+      </c>
+      <c r="C10" s="26">
         <v>1200</v>
       </c>
-      <c r="D10" s="27">
-        <v>1</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="D10" s="26">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="13"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="26">
-        <v>1</v>
-      </c>
-      <c r="C11" s="27">
+      <c r="B11" s="25">
+        <v>1</v>
+      </c>
+      <c r="C11" s="26">
         <v>1200</v>
       </c>
-      <c r="D11" s="27">
-        <v>1</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="26">
+        <v>1</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="13"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="26">
-        <v>1</v>
-      </c>
-      <c r="C12" s="27">
+      <c r="B12" s="25">
+        <v>1</v>
+      </c>
+      <c r="C12" s="26">
         <v>1200</v>
       </c>
-      <c r="D12" s="27">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="13"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="26">
-        <v>1</v>
-      </c>
-      <c r="C13" s="27">
+      <c r="B13" s="25">
+        <v>1</v>
+      </c>
+      <c r="C13" s="26">
         <v>1200</v>
       </c>
-      <c r="D13" s="27">
-        <v>1</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="26">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="32"/>
-      <c r="M13" s="13"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="31"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="34">
-        <v>1</v>
-      </c>
-      <c r="C14" s="35">
+      <c r="B14" s="33">
+        <v>1</v>
+      </c>
+      <c r="C14" s="34">
         <v>18000</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="34">
         <v>325</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="34">
-        <v>1</v>
-      </c>
-      <c r="C15" s="35">
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34">
         <v>18000</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="34">
         <v>325</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="20"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="34">
-        <v>1</v>
-      </c>
-      <c r="C16" s="35">
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="34">
         <v>15000</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="34">
         <v>280</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="34">
-        <v>1</v>
-      </c>
-      <c r="C17" s="35">
+      <c r="B17" s="33">
+        <v>1</v>
+      </c>
+      <c r="C17" s="34">
         <v>15000</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="34">
         <v>280</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="40">
         <v>100</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="34">
         <v>7000</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <v>90</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="H18" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="I18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="40">
         <v>100</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="34">
         <v>7000</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="34">
         <v>90</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="5"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="40">
         <v>100</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="34">
         <v>7000</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <v>90</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="5"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="33">
         <v>100</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="34">
         <v>5000</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <v>50</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="38" t="s">
+      <c r="H21" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="34">
-        <v>1</v>
-      </c>
-      <c r="C22" s="35">
+      <c r="B22" s="33">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34">
         <v>50000</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="34">
         <v>1300</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="5"/>
+      <c r="I22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="34">
-        <v>1</v>
-      </c>
-      <c r="C23" s="35">
+      <c r="B23" s="33">
+        <v>1</v>
+      </c>
+      <c r="C23" s="34">
         <v>40000</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="34">
         <v>900</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H23" s="38" t="s">
+      <c r="H23" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="20"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>100</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="26">
         <v>1800</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="26">
         <v>8</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
     </row>
     <row r="25" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="25">
         <v>100</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="26">
         <v>3000</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="26">
         <v>8</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="44">
         <v>100</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="45">
         <v>6500</v>
       </c>
-      <c r="D26" s="46">
+      <c r="D26" s="45">
         <v>235</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="H26" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="44">
+        <v>100</v>
+      </c>
+      <c r="C27" s="45">
+        <v>4500</v>
+      </c>
+      <c r="D27" s="45">
+        <v>170</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="45">
-        <v>0</v>
-      </c>
-      <c r="C27" s="46">
-        <v>4500</v>
-      </c>
-      <c r="D27" s="46">
-        <v>170</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="44" t="s">
+      <c r="H27" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="B28" s="51">
+        <v>1</v>
+      </c>
+      <c r="C28" s="52">
+        <v>15000</v>
+      </c>
+      <c r="D28" s="52">
+        <v>40</v>
+      </c>
+      <c r="E28" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="F28" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51" t="s">
+      <c r="G28" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="52">
-        <v>1</v>
-      </c>
-      <c r="C28" s="53">
-        <v>15000</v>
-      </c>
-      <c r="D28" s="53">
-        <v>40</v>
-      </c>
-      <c r="E28" s="54" t="s">
+      <c r="H28" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F28" s="51" t="s">
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="G28" s="55" t="s">
+      <c r="B29" s="51">
+        <v>1</v>
+      </c>
+      <c r="C29" s="52">
+        <v>4600</v>
+      </c>
+      <c r="D29" s="52">
+        <v>35</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="56" t="s">
+      <c r="G29" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="32"/>
-    </row>
-    <row r="29" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="H29" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="52">
-        <v>1</v>
-      </c>
-      <c r="C29" s="53">
-        <v>4600</v>
-      </c>
-      <c r="D29" s="53">
-        <v>35</v>
-      </c>
-      <c r="E29" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="51" t="s">
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="B30" s="51">
+        <v>1</v>
+      </c>
+      <c r="C30" s="52">
+        <v>16000</v>
+      </c>
+      <c r="D30" s="52">
+        <v>210</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="56" t="s">
+      <c r="G30" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="H30" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="52">
-        <v>1</v>
-      </c>
-      <c r="C30" s="53">
-        <v>16000</v>
-      </c>
-      <c r="D30" s="53">
-        <v>210</v>
-      </c>
-      <c r="E30" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="51" t="s">
+      <c r="I30" s="57"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="57"/>
+      <c r="N30" s="59"/>
+    </row>
+    <row r="31" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="B31" s="51">
+        <v>1</v>
+      </c>
+      <c r="C31" s="52">
+        <v>25000</v>
+      </c>
+      <c r="D31" s="52">
+        <v>265</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="H30" s="56" t="s">
+      <c r="G31" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="I30" s="58"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="58"/>
-      <c r="N30" s="60"/>
-    </row>
-    <row r="31" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
+      <c r="H31" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="52">
-        <v>1</v>
-      </c>
-      <c r="C31" s="53">
-        <v>25000</v>
-      </c>
-      <c r="D31" s="53">
-        <v>265</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="51" t="s">
+      <c r="I31" s="4"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="B32" s="51">
+        <v>1</v>
+      </c>
+      <c r="C32" s="52">
+        <v>4000</v>
+      </c>
+      <c r="D32" s="52">
+        <v>18</v>
+      </c>
+      <c r="E32" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="H31" s="56" t="s">
+      <c r="F32" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-    </row>
-    <row r="32" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51" t="s">
+      <c r="G32" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="52">
-        <v>1</v>
-      </c>
-      <c r="C32" s="53">
+      <c r="H32" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="51">
+        <v>1</v>
+      </c>
+      <c r="C33" s="52">
         <v>4000</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D33" s="52">
         <v>18</v>
       </c>
-      <c r="E32" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="61" t="s">
+      <c r="E33" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="H32" s="56" t="s">
+      <c r="G33" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="I33" s="4"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="11"/>
+    </row>
+    <row r="34" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="52">
-        <v>1</v>
-      </c>
-      <c r="C33" s="53">
+      <c r="B34" s="51">
+        <v>1</v>
+      </c>
+      <c r="C34" s="52">
         <v>4000</v>
       </c>
-      <c r="D33" s="53">
+      <c r="D34" s="52">
         <v>18</v>
       </c>
-      <c r="E33" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="51" t="s">
+      <c r="E34" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="G33" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="H33" s="56" t="s">
+      <c r="G34" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="I34" s="4"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="52">
-        <v>1</v>
-      </c>
-      <c r="C34" s="53">
+      <c r="B35" s="51">
+        <v>1</v>
+      </c>
+      <c r="C35" s="52">
         <v>4000</v>
       </c>
-      <c r="D34" s="53">
+      <c r="D35" s="52">
         <v>18</v>
       </c>
-      <c r="E34" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="51" t="s">
+      <c r="E35" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="G34" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="H34" s="56" t="s">
+      <c r="G35" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="H35" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="19"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="I34" s="5"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="51" t="s">
+      <c r="B36" s="2">
+        <v>100</v>
+      </c>
+      <c r="C36" s="3">
+        <v>9000</v>
+      </c>
+      <c r="D36" s="3">
+        <v>350</v>
+      </c>
+      <c r="E36" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="52">
-        <v>1</v>
-      </c>
-      <c r="C35" s="53">
-        <v>4000</v>
-      </c>
-      <c r="D35" s="53">
-        <v>18</v>
-      </c>
-      <c r="E35" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="51" t="s">
+      <c r="F36" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="G35" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" s="62" t="s">
-        <v>134</v>
-      </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="20"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="G36" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="B36" s="3">
-        <v>100</v>
-      </c>
-      <c r="C36" s="4">
-        <v>9000</v>
-      </c>
-      <c r="D36" s="4">
-        <v>350</v>
-      </c>
-      <c r="E36" s="64" t="s">
+      <c r="H36" s="65" t="s">
         <v>138</v>
-      </c>
-      <c r="F36" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="H36" s="66" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2204,7 +2211,7 @@
     <hyperlink ref="H24" r:id="rId21"/>
     <hyperlink ref="H25" r:id="rId22"/>
     <hyperlink ref="H26" r:id="rId23"/>
-    <hyperlink ref="H27" r:id="rId24"/>
+    <hyperlink ref="H27" r:id="rId24" display="..\..\Pictures\A TRABAJOS WEB\VELAS\COLORES Y AROMAS\Colores y aromas Rosas.jpg"/>
     <hyperlink ref="H28" r:id="rId25"/>
     <hyperlink ref="H29" r:id="rId26"/>
     <hyperlink ref="H30" r:id="rId27"/>

</xml_diff>

<commit_message>
Virgen de las Nieves
</commit_message>
<xml_diff>
--- a/data/web-repositorio.xlsx
+++ b/data/web-repositorio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="181">
   <si>
     <t>CARMELITAS BARILOCHE WEB</t>
   </si>
@@ -555,6 +555,18 @@
   </si>
   <si>
     <t>Esfera de Rosas</t>
+  </si>
+  <si>
+    <t>Cerámica Virgen de las Nieves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuestra Señora de las Nieves, imagen realizada en Cerámica con base de madera, 26,5 alto x 9,5 x 9,5. </t>
+  </si>
+  <si>
+    <t>..\Pictures\A TRABAJOS WEB\Cerámica\Virgen de las nieves.jpg</t>
+  </si>
+  <si>
+    <t>Virgen de las nieves</t>
   </si>
 </sst>
 </file>
@@ -806,7 +818,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -975,6 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3"/>
@@ -1239,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,7 +2152,7 @@
         <v>121</v>
       </c>
       <c r="B31" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="54">
         <v>25000</v>
@@ -2165,28 +2178,28 @@
     </row>
     <row r="32" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="B32" s="53">
         <v>1</v>
       </c>
       <c r="C32" s="54">
-        <v>4000</v>
+        <v>35000</v>
       </c>
       <c r="D32" s="54">
-        <v>18</v>
+        <v>495</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="H32" s="57" t="s">
-        <v>129</v>
+        <v>178</v>
+      </c>
+      <c r="H32" s="84" t="s">
+        <v>179</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="11"/>
@@ -2194,7 +2207,7 @@
     </row>
     <row r="33" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B33" s="53">
         <v>1</v>
@@ -2209,21 +2222,21 @@
         <v>126</v>
       </c>
       <c r="F33" s="52" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G33" s="62" t="s">
         <v>128</v>
       </c>
       <c r="H33" s="57" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="19"/>
+      <c r="J33" s="11"/>
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B34" s="53">
         <v>1</v>
@@ -2238,21 +2251,21 @@
         <v>126</v>
       </c>
       <c r="F34" s="52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G34" s="62" t="s">
         <v>128</v>
       </c>
       <c r="H34" s="57" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="10"/>
+      <c r="J34" s="19"/>
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B35" s="53">
         <v>1</v>
@@ -2267,81 +2280,83 @@
         <v>126</v>
       </c>
       <c r="F35" s="52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G35" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="H35" s="63" t="s">
+      <c r="H35" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="I35" s="48"/>
-      <c r="J35" s="11"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="11"/>
-      <c r="L35" s="19"/>
-    </row>
-    <row r="36" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+    </row>
+    <row r="36" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="53">
+        <v>1</v>
+      </c>
+      <c r="C36" s="54">
+        <v>4000</v>
+      </c>
+      <c r="D36" s="54">
+        <v>18</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="I36" s="48"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="19"/>
+    </row>
+    <row r="37" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
         <v>138</v>
-      </c>
-      <c r="B36" s="64">
-        <v>100</v>
-      </c>
-      <c r="C36" s="65">
-        <v>10000</v>
-      </c>
-      <c r="D36" s="66">
-        <v>350</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="G36" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="H36" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="I36" s="69"/>
-    </row>
-    <row r="37" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70" t="s">
-        <v>143</v>
       </c>
       <c r="B37" s="64">
         <v>100</v>
       </c>
-      <c r="C37" s="71">
-        <v>5800</v>
+      <c r="C37" s="65">
+        <v>10000</v>
       </c>
       <c r="D37" s="66">
-        <v>20</v>
+        <v>350</v>
       </c>
       <c r="E37" s="27" t="s">
         <v>139</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="G37" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="H37" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="I37" s="74"/>
+        <v>140</v>
+      </c>
+      <c r="G37" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" s="69"/>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
-        <v>147</v>
+      <c r="A38" s="70" t="s">
+        <v>143</v>
       </c>
       <c r="B38" s="64">
         <v>100</v>
       </c>
-      <c r="C38" s="66">
+      <c r="C38" s="71">
         <v>5800</v>
       </c>
       <c r="D38" s="66">
@@ -2351,44 +2366,45 @@
         <v>139</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G38" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="H38" s="75" t="s">
+      <c r="H38" s="73" t="s">
         <v>146</v>
       </c>
+      <c r="I38" s="74"/>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" s="77">
-        <v>1</v>
-      </c>
-      <c r="C39" s="78">
-        <v>10000</v>
-      </c>
-      <c r="D39" s="78">
-        <v>125</v>
-      </c>
-      <c r="E39" s="58" t="s">
-        <v>150</v>
-      </c>
-      <c r="F39" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="G39" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="H39" s="79" t="s">
-        <v>153</v>
+      <c r="A39" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="64">
+        <v>100</v>
+      </c>
+      <c r="C39" s="66">
+        <v>5800</v>
+      </c>
+      <c r="D39" s="66">
+        <v>20</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="H39" s="75" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B40" s="77">
         <v>1</v>
@@ -2403,44 +2419,44 @@
         <v>150</v>
       </c>
       <c r="F40" s="58" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G40" s="58" t="s">
         <v>152</v>
       </c>
       <c r="H40" s="79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="77">
+        <v>1</v>
+      </c>
+      <c r="C41" s="78">
+        <v>10000</v>
+      </c>
+      <c r="D41" s="78">
+        <v>125</v>
+      </c>
+      <c r="E41" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="G41" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="H41" s="79" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="80">
-        <v>1</v>
-      </c>
-      <c r="C41" s="81">
-        <v>9000</v>
-      </c>
-      <c r="D41" s="81">
-        <v>40</v>
-      </c>
-      <c r="E41" s="82" t="s">
-        <v>158</v>
-      </c>
-      <c r="F41" s="82" t="s">
-        <v>159</v>
-      </c>
-      <c r="G41" s="82" t="s">
-        <v>160</v>
-      </c>
-      <c r="H41" s="79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B42" s="80">
         <v>1</v>
@@ -2455,18 +2471,18 @@
         <v>158</v>
       </c>
       <c r="F42" s="82" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G42" s="82" t="s">
         <v>160</v>
       </c>
       <c r="H42" s="79" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B43" s="80">
         <v>1</v>
@@ -2481,18 +2497,18 @@
         <v>158</v>
       </c>
       <c r="F43" s="82" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G43" s="82" t="s">
         <v>160</v>
       </c>
       <c r="H43" s="79" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B44" s="80">
         <v>1</v>
@@ -2507,53 +2523,69 @@
         <v>158</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G44" s="82" t="s">
         <v>160</v>
       </c>
       <c r="H44" s="79" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="80">
+        <v>1</v>
+      </c>
+      <c r="C45" s="81">
+        <v>9000</v>
+      </c>
+      <c r="D45" s="81">
+        <v>40</v>
+      </c>
+      <c r="E45" s="82" t="s">
+        <v>158</v>
+      </c>
+      <c r="F45" s="82" t="s">
+        <v>169</v>
+      </c>
+      <c r="G45" s="82" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" s="79" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="80">
+      <c r="B46" s="80">
         <v>100</v>
       </c>
-      <c r="C45" s="81">
+      <c r="C46" s="81">
         <v>8000</v>
       </c>
-      <c r="D45" s="81">
+      <c r="D46" s="81">
         <v>250</v>
       </c>
-      <c r="E45" s="82" t="s">
+      <c r="E46" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="F45" s="82" t="s">
+      <c r="F46" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="G45" s="82" t="s">
+      <c r="G46" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="H45" s="79" t="s">
+      <c r="H46" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I46" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="82"/>
-      <c r="B46" s="80"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
     </row>
     <row r="47" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="82"/>
@@ -2564,6 +2596,16 @@
       <c r="F47" s="82"/>
       <c r="G47" s="82"/>
       <c r="H47" s="82"/>
+    </row>
+    <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="82"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2598,20 +2640,21 @@
     <hyperlink ref="H29" r:id="rId26"/>
     <hyperlink ref="H30" r:id="rId27"/>
     <hyperlink ref="H31" r:id="rId28"/>
-    <hyperlink ref="H32" r:id="rId29"/>
-    <hyperlink ref="H33" r:id="rId30"/>
-    <hyperlink ref="H34" r:id="rId31"/>
-    <hyperlink ref="H35" r:id="rId32"/>
-    <hyperlink ref="H36" r:id="rId33"/>
-    <hyperlink ref="H37" r:id="rId34"/>
-    <hyperlink ref="H38" r:id="rId35"/>
-    <hyperlink ref="H39" r:id="rId36"/>
-    <hyperlink ref="H40" r:id="rId37"/>
-    <hyperlink ref="H41" r:id="rId38"/>
-    <hyperlink ref="H42" r:id="rId39"/>
-    <hyperlink ref="H43" r:id="rId40"/>
-    <hyperlink ref="H44" r:id="rId41"/>
-    <hyperlink ref="H45" r:id="rId42"/>
+    <hyperlink ref="H33" r:id="rId29"/>
+    <hyperlink ref="H34" r:id="rId30"/>
+    <hyperlink ref="H35" r:id="rId31"/>
+    <hyperlink ref="H36" r:id="rId32"/>
+    <hyperlink ref="H37" r:id="rId33"/>
+    <hyperlink ref="H38" r:id="rId34"/>
+    <hyperlink ref="H39" r:id="rId35"/>
+    <hyperlink ref="H40" r:id="rId36"/>
+    <hyperlink ref="H41" r:id="rId37"/>
+    <hyperlink ref="H42" r:id="rId38"/>
+    <hyperlink ref="H43" r:id="rId39"/>
+    <hyperlink ref="H44" r:id="rId40"/>
+    <hyperlink ref="H45" r:id="rId41"/>
+    <hyperlink ref="H46" r:id="rId42"/>
+    <hyperlink ref="H32" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.39374999999999999" bottom="0.196527777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>